<commit_message>
Update Firebase Write DB and gitignore
</commit_message>
<xml_diff>
--- a/backend/resources/funeral_provider_directory.xlsx
+++ b/backend/resources/funeral_provider_directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b3268f5de74f2c5/Projects/funeral_services/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Efunero\backend\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{23696A3A-270E-4F67-8886-DBB2268DB84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59E23DF0-85C0-4D4B-B883-10EA506CF04D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E332E45-07F6-4A23-A263-809663717E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69E8DF15-8CD0-4CCC-A3DB-544871127071}"/>
+    <workbookView xWindow="-14505" yWindow="-1305" windowWidth="14610" windowHeight="15585" xr2:uid="{69E8DF15-8CD0-4CCC-A3DB-544871127071}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -301,6 +301,99 @@
   </si>
   <si>
     <t>https://www.vantaanhautaustoimisto.fi/hinnasto</t>
+  </si>
+  <si>
+    <t>Osoitteet_long</t>
+  </si>
+  <si>
+    <t>Mannerheimintie 65 Helsinki</t>
+  </si>
+  <si>
+    <t>Pihlajamäentie 32, Helsinki</t>
+  </si>
+  <si>
+    <t>Ulkoniitynkuja 6, Vantaa</t>
+  </si>
+  <si>
+    <t>Runeberginkatu 42,  Helsinki</t>
+  </si>
+  <si>
+    <t>Leppämäentie 2B, Espoo</t>
+  </si>
+  <si>
+    <t>Runeberginkatu 56, Helsinki</t>
+  </si>
+  <si>
+    <t>Kirkonkyläntie 14, Helsinki</t>
+  </si>
+  <si>
+    <t>Liisankatu 25, Helsinki;Vanhanlinnantie 3, Helsinki;Tapiontori 3C, Espoo;Ratatie 16, Vantaa</t>
+  </si>
+  <si>
+    <t>Mannerheimintie 45, Helsinki; Kielotie 4, Vantaa</t>
+  </si>
+  <si>
+    <t>Konstaapelinkatu 3, Espoo</t>
+  </si>
+  <si>
+    <t>Annankatu 12, Helsinki</t>
+  </si>
+  <si>
+    <t>Hiihtäjäntie 1, Helsinki</t>
+  </si>
+  <si>
+    <t>Mannerheimintie 69, Helsinki; Kirkonkyläntie 8, Helsinki</t>
+  </si>
+  <si>
+    <t>Palvelualue</t>
+  </si>
+  <si>
+    <t>Puhelinnumero</t>
+  </si>
+  <si>
+    <t>Huopalahdentie 3, Helsinki</t>
+  </si>
+  <si>
+    <t>09 488 140</t>
+  </si>
+  <si>
+    <t>040 940 1144</t>
+  </si>
+  <si>
+    <t>010 778 7777</t>
+  </si>
+  <si>
+    <t>020 732 0040</t>
+  </si>
+  <si>
+    <t>09 387 7659</t>
+  </si>
+  <si>
+    <t>09 448 346</t>
+  </si>
+  <si>
+    <t>0500 406 408</t>
+  </si>
+  <si>
+    <t>050 4727 980</t>
+  </si>
+  <si>
+    <t>020 155 5610;020 155 5612</t>
+  </si>
+  <si>
+    <t>09 686 261</t>
+  </si>
+  <si>
+    <t>010 231 3333;010 231 3331</t>
+  </si>
+  <si>
+    <t>09 7002 4824</t>
+  </si>
+  <si>
+    <t>09 7002 481</t>
+  </si>
+  <si>
+    <t>050 051 2942</t>
   </si>
 </sst>
 </file>
@@ -697,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8273688B-C045-4BDE-9386-3D7120F0B536}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,10 +802,14 @@
     <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="40.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="153.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="153.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="153.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -720,51 +817,45 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
       </c>
       <c r="G1" t="s">
         <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>66</v>
+      <c r="E2" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -774,14 +865,14 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -794,23 +885,20 @@
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4">
-        <v>784</v>
+      <c r="E4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>89</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -823,20 +911,14 @@
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F5">
-        <v>635</v>
+      <c r="E5" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -846,40 +928,40 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>75</v>
+      <c r="E6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" t="s">
         <v>35</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -889,20 +971,20 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
-        <v>77</v>
+      <c r="E8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -912,17 +994,17 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" t="s">
         <v>78</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -932,17 +1014,17 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" t="s">
         <v>42</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -955,23 +1037,20 @@
       <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11">
-        <v>907</v>
+      <c r="E11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" t="s">
+        <v>96</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -984,20 +1063,20 @@
       <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
-        <v>31</v>
+      <c r="E12" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" t="s">
+        <v>91</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1010,23 +1089,20 @@
       <c r="D13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13">
-        <v>980</v>
+      <c r="E13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1039,23 +1115,20 @@
       <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14">
-        <v>810</v>
+      <c r="E14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1065,35 +1138,30 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="E15" t="s">
-        <v>47</v>
+      <c r="E15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="G16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1103,17 +1171,14 @@
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
         <v>85</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1123,20 +1188,17 @@
       <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" t="s">
-        <v>53</v>
+      <c r="F18" t="s">
+        <v>100</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1149,14 +1211,8 @@
       <c r="G19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1167,7 +1223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -1178,7 +1234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1189,7 +1245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1200,7 +1256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1236,9 +1292,11 @@
     <hyperlink ref="G18" r:id="rId21" xr:uid="{753E486A-B3F2-46AB-BDD7-DB02C5135EC5}"/>
     <hyperlink ref="G19" r:id="rId22" xr:uid="{1F6073AE-CD25-403E-9CBA-DCDD9C25E270}"/>
     <hyperlink ref="G2" r:id="rId23" xr:uid="{3FCB6C1A-7829-4DD9-B816-497A1FBFFE3B}"/>
+    <hyperlink ref="B2" r:id="rId24" xr:uid="{52ACEE86-9D35-4845-B3F7-4A91F55D2529}"/>
+    <hyperlink ref="B7" r:id="rId25" xr:uid="{8369184A-41EB-4FCB-B76C-1E53C3383A86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -1246,7 +1304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381C8B94-87B1-4EA0-9E71-141F88D861BC}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix async of clean get response; correct naming of files and vars for clarity
</commit_message>
<xml_diff>
--- a/backend/resources/funeral_provider_directory.xlsx
+++ b/backend/resources/funeral_provider_directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Efunero\backend\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E332E45-07F6-4A23-A263-809663717E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107840C3-6293-4F24-9F93-05CE3E687243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="-1305" windowWidth="14610" windowHeight="15585" xr2:uid="{69E8DF15-8CD0-4CCC-A3DB-544871127071}"/>
+    <workbookView xWindow="-28920" yWindow="-1425" windowWidth="29040" windowHeight="15720" xr2:uid="{69E8DF15-8CD0-4CCC-A3DB-544871127071}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -252,9 +252,6 @@
     <t>https://hautaustoimistobieder.fi/peruspaketti-hautajaisten-jarjestamiseen/;https://hautaustoimistobieder.fi/uurnat/;https://hautaustoimistobieder.fi/kukat-hautajaisiin/</t>
   </si>
   <si>
-    <t>https://hautaustoimistotoro.fi/suoratuhkaus-hautajaispaketti/; https://hautaustoimistotoro.fi/surukukat/;https://hautaustoimistotoro.fi/arkkukuljetukset/</t>
-  </si>
-  <si>
     <t>hasOffice</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>050 051 2942</t>
+  </si>
+  <si>
+    <t>https://hautaustoimistotoro.fi/suoratuhkaus-hautajaispaketti/; https://hautaustoimistotoro.fi/surukukat/;https://hautaustoimistotoro.fi/arkkukuljetukset/;https://hautaustoimistotoro.fi/uurnat/</t>
   </si>
 </sst>
 </file>
@@ -793,7 +793,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,13 +817,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s">
         <v>30</v>
@@ -832,7 +832,7 @@
         <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>65</v>
@@ -866,10 +866,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -886,16 +886,16 @@
         <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -912,10 +912,10 @@
         <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,16 +929,16 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
         <v>74</v>
-      </c>
-      <c r="H6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,10 +952,10 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
         <v>35</v>
@@ -972,16 +972,16 @@
         <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
         <v>76</v>
-      </c>
-      <c r="H8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -995,13 +995,13 @@
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1015,10 +1015,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -1038,13 +1038,13 @@
         <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
         <v>37</v>
@@ -1064,13 +1064,13 @@
         <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1090,13 +1090,13 @@
         <v>32</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -1116,13 +1116,13 @@
         <v>40</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" t="s">
         <v>41</v>
@@ -1139,13 +1139,13 @@
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" t="s">
         <v>47</v>
@@ -1172,10 +1172,10 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1189,10 +1189,10 @@
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
         <v>53</v>
@@ -1209,7 +1209,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,7 +1339,7 @@
         <v>69</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
         <v>907</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1383,10 +1383,10 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3">
         <v>1</v>

</xml_diff>